<commit_message>
changes for ui integration
</commit_message>
<xml_diff>
--- a/src/main/resources/static/export/template/EMPLOYEE_DATA.xlsx
+++ b/src/main/resources/static/export/template/EMPLOYEE_DATA.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>EMP_ID</t>
   </si>
@@ -39,9 +40,6 @@
     <t>SSC.VRAMASAMY</t>
   </si>
   <si>
-    <t>IS_RM</t>
-  </si>
-  <si>
     <t>RM_NAME</t>
   </si>
   <si>
@@ -61,6 +59,12 @@
   </si>
   <si>
     <t>SSC.VRAMASAMY@CMA-CGM.COM</t>
+  </si>
+  <si>
+    <t>IS_ADMIN</t>
+  </si>
+  <si>
+    <t>EMAIL_ID</t>
   </si>
 </sst>
 </file>
@@ -410,115 +414,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.5703125" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="64.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4780</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5348</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3666</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4334</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="b">
+      <c r="F5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4734</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="b">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="D2" r:id="rId5"/>
-    <hyperlink ref="D3" r:id="rId6"/>
-    <hyperlink ref="D4" r:id="rId7"/>
-    <hyperlink ref="D5" r:id="rId8"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="E2" r:id="rId5"/>
+    <hyperlink ref="E3" r:id="rId6"/>
+    <hyperlink ref="E4" r:id="rId7"/>
+    <hyperlink ref="E5" r:id="rId8"/>
+    <hyperlink ref="B6" r:id="rId9"/>
+    <hyperlink ref="E6" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes for team name added , pagination added active time page , task timer page multiple select removed and moved above of the table
</commit_message>
<xml_diff>
--- a/src/main/resources/static/export/template/EMPLOYEE_DATA.xlsx
+++ b/src/main/resources/static/export/template/EMPLOYEE_DATA.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>EMP_ID</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>IS_ACTIVE</t>
+  </si>
+  <si>
+    <t>TEAM_NAME</t>
+  </si>
+  <si>
+    <t>IT/ARCHTECH</t>
+  </si>
+  <si>
+    <t>IT</t>
   </si>
 </sst>
 </file>
@@ -447,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +470,7 @@
     <col min="5" max="5" width="64.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,8 +492,11 @@
       <c r="G1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4780</v>
       </c>
@@ -506,8 +518,11 @@
       <c r="G2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5348</v>
       </c>
@@ -529,8 +544,11 @@
       <c r="G3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3666</v>
       </c>
@@ -552,8 +570,11 @@
       <c r="G4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4334</v>
       </c>
@@ -575,8 +596,11 @@
       <c r="G5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4734</v>
       </c>
@@ -598,8 +622,11 @@
       <c r="G6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1001</v>
       </c>
@@ -621,8 +648,11 @@
       <c r="G7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1002</v>
       </c>
@@ -644,8 +674,11 @@
       <c r="G8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3001</v>
       </c>
@@ -667,8 +700,11 @@
       <c r="G9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2001</v>
       </c>
@@ -690,8 +726,11 @@
       <c r="G10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2002</v>
       </c>
@@ -712,6 +751,9 @@
       </c>
       <c r="G11" t="b">
         <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
column name changed in template. RM_ID AS RM_EMAIL_ID
</commit_message>
<xml_diff>
--- a/src/main/resources/static/export/template/EMPLOYEE_DATA.xlsx
+++ b/src/main/resources/static/export/template/EMPLOYEE_DATA.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7740"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="13890" windowHeight="6360"/>
   </bookViews>
   <sheets>
     <sheet name="EmployeeDetails" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -40,9 +41,6 @@
     <t>SSC.VRAMASAMY</t>
   </si>
   <si>
-    <t>RM_NAME</t>
-  </si>
-  <si>
     <t>RM_ID</t>
   </si>
   <si>
@@ -107,6 +105,9 @@
   </si>
   <si>
     <t>IT</t>
+  </si>
+  <si>
+    <t>RM_EMAIL_ID</t>
   </si>
 </sst>
 </file>
@@ -459,7 +460,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +476,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -484,16 +485,16 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -501,7 +502,7 @@
         <v>4780</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -509,17 +510,17 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -527,7 +528,7 @@
         <v>5348</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -535,8 +536,8 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
-        <v>3</v>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -545,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -553,7 +554,7 @@
         <v>3666</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -561,8 +562,8 @@
       <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>3</v>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -571,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -579,7 +580,7 @@
         <v>4334</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -587,8 +588,8 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>6</v>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -597,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -605,7 +606,7 @@
         <v>4734</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -613,8 +614,8 @@
       <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
-        <v>6</v>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -623,7 +624,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -631,17 +632,17 @@
         <v>1001</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
@@ -649,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -657,17 +658,17 @@
         <v>1002</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
       <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
       <c r="F8" t="b">
         <v>0</v>
       </c>
@@ -675,7 +676,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -683,25 +684,25 @@
         <v>3001</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -709,17 +710,17 @@
         <v>2001</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
@@ -727,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -735,17 +736,17 @@
         <v>2002</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
@@ -753,7 +754,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -768,6 +769,16 @@
     <hyperlink ref="B10" r:id="rId8"/>
     <hyperlink ref="B9" r:id="rId9"/>
     <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="E2" r:id="rId11"/>
+    <hyperlink ref="E3" r:id="rId12"/>
+    <hyperlink ref="E4" r:id="rId13"/>
+    <hyperlink ref="E5" r:id="rId14"/>
+    <hyperlink ref="E6" r:id="rId15"/>
+    <hyperlink ref="E7" r:id="rId16"/>
+    <hyperlink ref="E8" r:id="rId17"/>
+    <hyperlink ref="E9" r:id="rId18"/>
+    <hyperlink ref="E10" r:id="rId19"/>
+    <hyperlink ref="E11" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>